<commit_message>
Melhorias no layout da lpd da Genese
</commit_message>
<xml_diff>
--- a/client_data/gns/ldp.xlsx
+++ b/client_data/gns/ldp.xlsx
@@ -66,10 +66,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="24">
     <font>
@@ -110,6 +110,98 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FF9C6500"/>
       <name val="Calibri"/>
@@ -118,22 +210,21 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -147,33 +238,11 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -184,75 +253,6 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="34">
     <fill>
@@ -269,55 +269,157 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -329,127 +431,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -463,17 +463,26 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FF3F3F3F"/>
       </left>
       <right style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FF3F3F3F"/>
       </right>
       <top style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FF3F3F3F"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -482,7 +491,7 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4"/>
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -502,11 +511,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -531,21 +546,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="double">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -565,156 +565,162 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="3" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="10" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="10" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="29" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="32" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1">
@@ -724,7 +730,7 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+      <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
@@ -800,8 +806,8 @@
     <xdr:to>
       <xdr:col>1</xdr:col>
       <xdr:colOff>1896745</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>65405</xdr:rowOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>68580</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1093,7 +1099,7 @@
   <dimension ref="A1:L9"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.8" defaultRowHeight="12.75"/>
@@ -1107,92 +1113,95 @@
     <col min="7" max="7" width="12.9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="46" customHeight="1" spans="3:7">
-      <c r="C1" s="1"/>
-      <c r="G1" s="4" t="s">
+    <row r="1" s="1" customFormat="1" ht="33" customHeight="1" spans="3:7">
+      <c r="C1" s="2"/>
+      <c r="G1" s="6" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="2" ht="18" customHeight="1" spans="7:7">
-      <c r="G2" s="5" t="s">
+      <c r="G2" s="7" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="3" ht="15" customHeight="1"/>
+    <row r="4" spans="2:2">
+      <c r="B4" s="3"/>
+    </row>
     <row r="5" spans="1:12">
-      <c r="A5" s="2" t="s">
+      <c r="A5" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="2"/>
-      <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2"/>
-      <c r="F5" s="2"/>
-      <c r="G5" s="6" t="s">
+      <c r="B5" s="4"/>
+      <c r="C5" s="4"/>
+      <c r="D5" s="4"/>
+      <c r="E5" s="4"/>
+      <c r="F5" s="4"/>
+      <c r="G5" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="H5" s="2"/>
-      <c r="I5" s="2"/>
-      <c r="J5" s="2"/>
-      <c r="K5" s="2"/>
-      <c r="L5" s="2"/>
+      <c r="H5" s="4"/>
+      <c r="I5" s="4"/>
+      <c r="J5" s="4"/>
+      <c r="K5" s="4"/>
+      <c r="L5" s="4"/>
     </row>
     <row r="6" spans="1:12">
-      <c r="A6" s="2" t="s">
+      <c r="A6" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="2"/>
-      <c r="C6" s="2"/>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2"/>
-      <c r="F6" s="2"/>
-      <c r="G6" s="6" t="s">
+      <c r="B6" s="4"/>
+      <c r="C6" s="4"/>
+      <c r="D6" s="4"/>
+      <c r="E6" s="4"/>
+      <c r="F6" s="4"/>
+      <c r="G6" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="H6" s="2"/>
-      <c r="I6" s="2"/>
-      <c r="J6" s="2"/>
-      <c r="K6" s="2"/>
-      <c r="L6" s="2"/>
+      <c r="H6" s="4"/>
+      <c r="I6" s="4"/>
+      <c r="J6" s="4"/>
+      <c r="K6" s="4"/>
+      <c r="L6" s="4"/>
     </row>
     <row r="7" spans="1:12">
-      <c r="A7" s="2" t="s">
+      <c r="A7" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="2"/>
-      <c r="C7" s="2"/>
-      <c r="D7" s="2"/>
-      <c r="E7" s="2"/>
-      <c r="F7" s="2"/>
-      <c r="G7" s="6" t="s">
+      <c r="B7" s="4"/>
+      <c r="C7" s="4"/>
+      <c r="D7" s="4"/>
+      <c r="E7" s="4"/>
+      <c r="F7" s="4"/>
+      <c r="G7" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="H7" s="2"/>
-      <c r="I7" s="2"/>
-      <c r="J7" s="2"/>
-      <c r="K7" s="2"/>
-      <c r="L7" s="2"/>
+      <c r="H7" s="4"/>
+      <c r="I7" s="4"/>
+      <c r="J7" s="4"/>
+      <c r="K7" s="4"/>
+      <c r="L7" s="4"/>
     </row>
     <row r="9" ht="21" customHeight="1" spans="1:7">
-      <c r="A9" s="3" t="s">
+      <c r="A9" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="3" t="s">
+      <c r="B9" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C9" s="3" t="s">
+      <c r="C9" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="D9" s="3" t="s">
+      <c r="D9" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="E9" s="3" t="s">
+      <c r="E9" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="F9" s="3" t="s">
+      <c r="F9" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="G9" s="3" t="s">
+      <c r="G9" s="5" t="s">
         <v>14</v>
       </c>
     </row>

</xml_diff>